<commit_message>
[analysis] wip: add UI
</commit_message>
<xml_diff>
--- a/O4/YeuCau/YeuCau.xlsx
+++ b/O4/YeuCau/YeuCau.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0A0E8BC0-76F3-4FFF-8D8E-5275C7F89481}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>STT</t>
   </si>
@@ -35,12 +36,30 @@
   </si>
   <si>
     <t>abc( string id, out List&lt;BenhNhan&gt; lstBenhNhan)</t>
+  </si>
+  <si>
+    <t>Sửa hàm DangNhapProcess ở DangNhapModule</t>
+  </si>
+  <si>
+    <t>App crash khi đăng nhập fail</t>
+  </si>
+  <si>
+    <t>Sửa hàm getPhong ở màn hình tiếp nhận</t>
+  </si>
+  <si>
+    <t>Ở màn hình tiếp nhận, hàm getPhong chỉ mong muốn get ra những phòng khám, ko có phòng tiếp nhận và phòng xét nghiệm</t>
+  </si>
+  <si>
+    <t>Thêm Function GetInformationBenhNhan ở Module XetNghiem</t>
+  </si>
+  <si>
+    <t>GetInformationBenhNhan(string MaBenhNhan, out BenhNhanDTO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,22 +136,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -227,6 +258,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -262,6 +310,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,113 +502,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="64.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="45.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="64.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "[analysis] wip: add UI"
This reverts commit bb89a717bdf1f13a61c5a6385e8f6780932166ef.
</commit_message>
<xml_diff>
--- a/O4/YeuCau/YeuCau.xlsx
+++ b/O4/YeuCau/YeuCau.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0A0E8BC0-76F3-4FFF-8D8E-5275C7F89481}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>STT</t>
   </si>
@@ -36,30 +35,12 @@
   </si>
   <si>
     <t>abc( string id, out List&lt;BenhNhan&gt; lstBenhNhan)</t>
-  </si>
-  <si>
-    <t>Sửa hàm DangNhapProcess ở DangNhapModule</t>
-  </si>
-  <si>
-    <t>App crash khi đăng nhập fail</t>
-  </si>
-  <si>
-    <t>Sửa hàm getPhong ở màn hình tiếp nhận</t>
-  </si>
-  <si>
-    <t>Ở màn hình tiếp nhận, hàm getPhong chỉ mong muốn get ra những phòng khám, ko có phòng tiếp nhận và phòng xét nghiệm</t>
-  </si>
-  <si>
-    <t>Thêm Function GetInformationBenhNhan ở Module XetNghiem</t>
-  </si>
-  <si>
-    <t>GetInformationBenhNhan(string MaBenhNhan, out BenhNhanDTO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,34 +117,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -258,23 +227,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -310,23 +262,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -502,133 +437,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="45.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="64.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>